<commit_message>
Edited some inputs, but still need temperature range and electrical input
</commit_message>
<xml_diff>
--- a/Input/Planet_Values.xlsx
+++ b/Input/Planet_Values.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e03eb733b9ff670a/Documents/Adam's School Work/Aero 582/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e03eb733b9ff670a/Documents/Adam's School Work/Aero 582 583/UMBRA-Thermal/Input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{9DDDBB59-6E39-49E4-AC5F-5ED46BA25771}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3A27F6A1-6CCB-4629-BB02-0CFB5F46AC7A}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="13_ncr:1_{9DDDBB59-6E39-49E4-AC5F-5ED46BA25771}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B86481CD-734C-4391-9C71-C7D812614CCD}"/>
   <bookViews>
-    <workbookView xWindow="7095" yWindow="1020" windowWidth="21600" windowHeight="11385" xr2:uid="{36F17989-3586-447C-92AC-1E9958DF48F7}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" xr2:uid="{36F17989-3586-447C-92AC-1E9958DF48F7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>Mass (kg)</t>
   </si>
@@ -85,6 +85,15 @@
   </si>
   <si>
     <t>Altitude Input (km)</t>
+  </si>
+  <si>
+    <t>Red Color</t>
+  </si>
+  <si>
+    <t>Blue Color</t>
+  </si>
+  <si>
+    <t>Green Color</t>
   </si>
 </sst>
 </file>
@@ -454,23 +463,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A958C82-9A04-4010-9331-177F67D9326E}">
-  <dimension ref="A1:Q22"/>
+  <dimension ref="A1:T22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M7" sqref="M7"/>
+      <selection activeCell="S1" sqref="S1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.33203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
     <col min="8" max="9" width="10" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17">
+    <row r="1" spans="1:20">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -519,8 +528,17 @@
       <c r="Q1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="2" spans="1:17">
+      <c r="R1" t="s">
+        <v>20</v>
+      </c>
+      <c r="S1" t="s">
+        <v>21</v>
+      </c>
+      <c r="T1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -577,8 +595,20 @@
       <c r="Q2" s="2">
         <v>7800</v>
       </c>
-    </row>
-    <row r="3" spans="1:17">
+      <c r="R2">
+        <f>(139+187+221+239)/4/255</f>
+        <v>0.77058823529411768</v>
+      </c>
+      <c r="S2">
+        <f>(145+183+216+239)/4/255</f>
+        <v>0.76764705882352946</v>
+      </c>
+      <c r="T2">
+        <f>(161+171+212+239)/4/255</f>
+        <v>0.76764705882352946</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -633,10 +663,22 @@
         <v>100.46435</v>
       </c>
       <c r="Q3" s="2">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17">
+        <v>1000</v>
+      </c>
+      <c r="R3">
+        <f>(5+11+227+161+178+127)/6/255</f>
+        <v>0.46339869281045754</v>
+      </c>
+      <c r="S3">
+        <f>(51+158+197+110+189+139)/6/255</f>
+        <v>0.5516339869281045</v>
+      </c>
+      <c r="T3">
+        <f>(85+210+117+71+91+59)/6/255</f>
+        <v>0.4137254901960784</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -693,8 +735,20 @@
       <c r="Q4" s="2">
         <v>16000000</v>
       </c>
-    </row>
-    <row r="5" spans="1:17">
+      <c r="R4">
+        <f>(64+167+210+211+144+200)/6/255</f>
+        <v>0.65098039215686276</v>
+      </c>
+      <c r="S4">
+        <f>(68+156+207+156+97+139)/6/255</f>
+        <v>0.53790849673202612</v>
+      </c>
+      <c r="T4">
+        <f>(54+134+218+126+77+58)/6/255</f>
+        <v>0.43594771241830066</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -752,38 +806,50 @@
         <f>1.5*C5*10^-3</f>
         <v>38338.5</v>
       </c>
-    </row>
-    <row r="6" spans="1:17">
+      <c r="R5">
+        <f>(213+187+147+101)/4/255</f>
+        <v>0.63529411764705879</v>
+      </c>
+      <c r="S5">
+        <f>(251+225+184+134)/4/255</f>
+        <v>0.77843137254901962</v>
+      </c>
+      <c r="T5">
+        <f>(252+228+190+139)/4/255</f>
+        <v>0.79313725490196074</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20">
       <c r="A6" s="1"/>
     </row>
-    <row r="7" spans="1:17">
+    <row r="7" spans="1:20">
       <c r="A7" s="1"/>
     </row>
-    <row r="8" spans="1:17">
+    <row r="8" spans="1:20">
       <c r="A8" s="1"/>
     </row>
-    <row r="9" spans="1:17">
+    <row r="9" spans="1:20">
       <c r="A9" s="1"/>
     </row>
-    <row r="10" spans="1:17">
+    <row r="10" spans="1:20">
       <c r="A10" s="1"/>
     </row>
-    <row r="11" spans="1:17">
+    <row r="11" spans="1:20">
       <c r="A11" s="1"/>
     </row>
-    <row r="12" spans="1:17">
+    <row r="12" spans="1:20">
       <c r="A12" s="1"/>
     </row>
-    <row r="13" spans="1:17">
+    <row r="13" spans="1:20">
       <c r="A13" s="1"/>
     </row>
-    <row r="14" spans="1:17">
+    <row r="14" spans="1:20">
       <c r="A14" s="1"/>
     </row>
-    <row r="15" spans="1:17">
+    <row r="15" spans="1:20">
       <c r="A15" s="1"/>
     </row>
-    <row r="16" spans="1:17">
+    <row r="16" spans="1:20">
       <c r="A16" s="1"/>
     </row>
     <row r="17" spans="1:1">

</xml_diff>

<commit_message>
change to the earth altitude
</commit_message>
<xml_diff>
--- a/Input/Planet_Values.xlsx
+++ b/Input/Planet_Values.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e03eb733b9ff670a/Documents/Adam's School Work/Aero 582 583/UMBRA-Thermal/Input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="13_ncr:1_{9DDDBB59-6E39-49E4-AC5F-5ED46BA25771}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B86481CD-734C-4391-9C71-C7D812614CCD}"/>
+  <xr:revisionPtr revIDLastSave="7" documentId="13_ncr:1_{9DDDBB59-6E39-49E4-AC5F-5ED46BA25771}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A5351C05-E8FA-43CD-9BF5-CB2F8835B316}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" xr2:uid="{36F17989-3586-447C-92AC-1E9958DF48F7}"/>
+    <workbookView xWindow="6750" yWindow="675" windowWidth="21600" windowHeight="11385" xr2:uid="{36F17989-3586-447C-92AC-1E9958DF48F7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -465,18 +465,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A958C82-9A04-4010-9331-177F67D9326E}">
   <dimension ref="A1:T22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S1" sqref="S1"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="Q4" sqref="Q4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
     <col min="8" max="9" width="10" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20">
@@ -663,7 +663,7 @@
         <v>100.46435</v>
       </c>
       <c r="Q3" s="2">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="R3">
         <f>(5+11+227+161+178+127)/6/255</f>

</xml_diff>

<commit_message>
fixed some issues with pi
</commit_message>
<xml_diff>
--- a/Input/Planet_Values.xlsx
+++ b/Input/Planet_Values.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e03eb733b9ff670a/Documents/Adam's School Work/Aero 582 583/UMBRA-Thermal/Input/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Adam\OneDrive\Documents\Adam's School Work\Aero 582 583\UMBRA-Thermal\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="7" documentId="13_ncr:1_{9DDDBB59-6E39-49E4-AC5F-5ED46BA25771}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A5351C05-E8FA-43CD-9BF5-CB2F8835B316}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FCA0A88-1960-40A6-BE2F-994417782A5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6750" yWindow="675" windowWidth="21600" windowHeight="11385" xr2:uid="{36F17989-3586-447C-92AC-1E9958DF48F7}"/>
   </bookViews>

</xml_diff>